<commit_message>
SOLAR_GRANULATION_RMS = 0.8;  fixed binder loading
</commit_message>
<xml_diff>
--- a/results/GAIA_TESS_candidate_matches.xlsx
+++ b/results/GAIA_TESS_candidate_matches.xlsx
@@ -622,7 +622,7 @@
         <v>0.618173</v>
       </c>
       <c r="Q2" s="3" t="n">
-        <v>0.4644199760795594</v>
+        <v>0.8239175227358072</v>
       </c>
       <c r="R2" t="n">
         <v>0.1536852942719399</v>
@@ -678,7 +678,7 @@
         <v>0.639371</v>
       </c>
       <c r="Q3" s="3" t="n">
-        <v>0.6217175629236638</v>
+        <v>1.086836000081502</v>
       </c>
       <c r="R3" t="n">
         <v>0.08762883918922149</v>
@@ -734,7 +734,7 @@
         <v>0.603336</v>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>0.9621770088035774</v>
+        <v>1.673011684280936</v>
       </c>
       <c r="R4" t="n">
         <v>0.08879781148820186</v>
@@ -790,7 +790,7 @@
         <v>0.7017099999999999</v>
       </c>
       <c r="Q5" s="3" t="n">
-        <v>0.6595363756557957</v>
+        <v>1.155518363889651</v>
       </c>
       <c r="R5" t="n">
         <v>0.01821666933803688</v>
@@ -846,7 +846,7 @@
         <v>0.661076</v>
       </c>
       <c r="Q6" s="3" t="n">
-        <v>0.5078596040079951</v>
+        <v>0.8995655422072516</v>
       </c>
       <c r="R6" t="n">
         <v>0.07410788918668496</v>
@@ -902,7 +902,7 @@
         <v>0.66</v>
       </c>
       <c r="Q7" s="3" t="n">
-        <v>0.5078596040079951</v>
+        <v>0.8995655422072516</v>
       </c>
       <c r="R7" t="n">
         <v>0.07410788918668496</v>
@@ -958,7 +958,7 @@
         <v>0.7210839999999999</v>
       </c>
       <c r="Q8" s="3" t="n">
-        <v>0.935961884875647</v>
+        <v>1.639734192087474</v>
       </c>
       <c r="R8" t="n">
         <v>0.04720909237717162</v>
@@ -1014,7 +1014,7 @@
         <v>0.626722</v>
       </c>
       <c r="Q9" s="3" t="n">
-        <v>1.066521483154316</v>
+        <v>1.855414867436865</v>
       </c>
       <c r="R9" t="n">
         <v>0.05933370243670238</v>
@@ -1070,7 +1070,7 @@
         <v>0.6750930000000001</v>
       </c>
       <c r="Q10" s="3" t="n">
-        <v>0.8304488523779201</v>
+        <v>1.44974443522691</v>
       </c>
       <c r="R10" t="n">
         <v>0.04566165863559627</v>
@@ -1126,7 +1126,7 @@
         <v>0.636572</v>
       </c>
       <c r="Q11" s="3" t="n">
-        <v>1.446091471842279</v>
+        <v>2.511247632757248</v>
       </c>
       <c r="R11" t="n">
         <v>0.07251061220725062</v>
@@ -1182,7 +1182,7 @@
         <v>0.6634139999999999</v>
       </c>
       <c r="Q12" s="3" t="n">
-        <v>0.9223986185530643</v>
+        <v>1.607880801785313</v>
       </c>
       <c r="R12" t="n">
         <v>0.04285830752449767</v>
@@ -1238,7 +1238,7 @@
         <v>0.732115</v>
       </c>
       <c r="Q13" s="3" t="n">
-        <v>0.5875221654235464</v>
+        <v>1.04713564664033</v>
       </c>
       <c r="R13" t="n">
         <v>0.1818675256393356</v>
@@ -1294,7 +1294,7 @@
         <v>0.63</v>
       </c>
       <c r="Q14" s="3" t="n">
-        <v>0.7573579347875248</v>
+        <v>1.326232586610272</v>
       </c>
       <c r="R14" t="n">
         <v>0.2166081726537622</v>
@@ -1350,7 +1350,7 @@
         <v>0.617519</v>
       </c>
       <c r="Q15" s="3" t="n">
-        <v>1.142903089246784</v>
+        <v>1.98896214143939</v>
       </c>
       <c r="R15" t="n">
         <v>0.1945912951651126</v>
@@ -1406,7 +1406,7 @@
         <v>0.71</v>
       </c>
       <c r="Q16" s="3" t="n">
-        <v>0.3840778462287892</v>
+        <v>0.7360760259646952</v>
       </c>
       <c r="R16" t="n">
         <v>0.216873501781118</v>
@@ -1462,7 +1462,7 @@
         <v>0.71</v>
       </c>
       <c r="Q17" s="3" t="n">
-        <v>0.3840778462287892</v>
+        <v>0.7360760259646952</v>
       </c>
       <c r="R17" t="n">
         <v>0.216873501781118</v>
@@ -1518,7 +1518,7 @@
         <v>0.590924</v>
       </c>
       <c r="Q18" s="3" t="n">
-        <v>1.54172749561661</v>
+        <v>2.674574616230561</v>
       </c>
       <c r="R18" t="n">
         <v>0.1022963165103159</v>
@@ -1574,7 +1574,7 @@
         <v>0.700727</v>
       </c>
       <c r="Q19" s="3" t="n">
-        <v>0.9769186864503394</v>
+        <v>1.711840798525595</v>
       </c>
       <c r="R19" t="n">
         <v>0.02144133416206292</v>
@@ -1630,7 +1630,7 @@
         <v>0.701499</v>
       </c>
       <c r="Q20" s="3" t="n">
-        <v>0.4464933530419892</v>
+        <v>0.8422036146915931</v>
       </c>
       <c r="R20" t="n">
         <v>0.2489958576576189</v>
@@ -1686,7 +1686,7 @@
         <v>0.622512</v>
       </c>
       <c r="Q21" s="3" t="n">
-        <v>0.8895167524026653</v>
+        <v>1.567080541948636</v>
       </c>
       <c r="R21" t="n">
         <v>0.2100230324201724</v>
@@ -1742,7 +1742,7 @@
         <v>0.630715</v>
       </c>
       <c r="Q22" s="3" t="n">
-        <v>0.3183878703705095</v>
+        <v>0.6036502700178147</v>
       </c>
       <c r="R22" t="n">
         <v>0.3529309609610866</v>
@@ -1798,7 +1798,7 @@
         <v>0.630715</v>
       </c>
       <c r="Q23" s="3" t="n">
-        <v>0.3183878703705095</v>
+        <v>0.6036502700178147</v>
       </c>
       <c r="R23" t="n">
         <v>0.3529309609610866</v>
@@ -1854,7 +1854,7 @@
         <v>0.630715</v>
       </c>
       <c r="Q24" s="3" t="n">
-        <v>0.3183878703705095</v>
+        <v>0.6036502700178147</v>
       </c>
       <c r="R24" t="n">
         <v>0.3529309609610866</v>
@@ -1910,7 +1910,7 @@
         <v>0.71</v>
       </c>
       <c r="Q25" s="3" t="n">
-        <v>0.9308156236180681</v>
+        <v>1.645503504737809</v>
       </c>
       <c r="R25" t="n">
         <v>0.1214124615862055</v>
@@ -1966,7 +1966,7 @@
         <v>0.75</v>
       </c>
       <c r="Q26" s="3" t="n">
-        <v>0.4686604135697814</v>
+        <v>0.8663687244288396</v>
       </c>
       <c r="R26" t="n">
         <v>0.03576864546243089</v>
@@ -2022,7 +2022,7 @@
         <v>0.678033</v>
       </c>
       <c r="Q27" s="3" t="n">
-        <v>0.8070233188124741</v>
+        <v>1.429141886451972</v>
       </c>
       <c r="R27" t="n">
         <v>0.03672621597918261</v>
@@ -2078,7 +2078,7 @@
         <v>0.68</v>
       </c>
       <c r="Q28" s="3" t="n">
-        <v>1.239403332584826</v>
+        <v>2.167290027842529</v>
       </c>
       <c r="R28" t="n">
         <v>0.1915281956726753</v>
@@ -2134,7 +2134,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="Q29" s="3" t="n">
-        <v>0.4369855154896619</v>
+        <v>0.8066475768186987</v>
       </c>
       <c r="R29" t="n">
         <v>0.2060338426977061</v>
@@ -2190,7 +2190,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="Q30" s="3" t="n">
-        <v>0.7830204577516093</v>
+        <v>1.390642899182112</v>
       </c>
       <c r="R30" t="n">
         <v>0.05462548793553362</v>
@@ -2246,7 +2246,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="Q31" s="3" t="n">
-        <v>0.7830204577516093</v>
+        <v>1.390642899182112</v>
       </c>
       <c r="R31" t="n">
         <v>0.05462548793553362</v>
@@ -2302,7 +2302,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="Q32" s="3" t="n">
-        <v>0.7830204577516093</v>
+        <v>1.390642899182112</v>
       </c>
       <c r="R32" t="n">
         <v>0.05462548793553362</v>
@@ -2358,7 +2358,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="Q33" s="3" t="n">
-        <v>0.7830204577516093</v>
+        <v>1.390642899182112</v>
       </c>
       <c r="R33" t="n">
         <v>0.05462548793553362</v>
@@ -2414,7 +2414,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="Q34" s="3" t="n">
-        <v>0.7830204577516093</v>
+        <v>1.390642899182112</v>
       </c>
       <c r="R34" t="n">
         <v>0.05462548793553362</v>
@@ -2470,7 +2470,7 @@
         <v>0.750709</v>
       </c>
       <c r="Q35" s="3" t="n">
-        <v>0.4877356136941862</v>
+        <v>0.9117968498801516</v>
       </c>
       <c r="R35" t="n">
         <v>0.08153377876240343</v>
@@ -2526,7 +2526,7 @@
         <v>0.76</v>
       </c>
       <c r="Q36" s="3" t="n">
-        <v>0.8755490982267587</v>
+        <v>1.559962907000137</v>
       </c>
       <c r="R36" t="n">
         <v>0.01321577041923607</v>
@@ -2582,7 +2582,7 @@
         <v>0.7266319999999999</v>
       </c>
       <c r="Q37" s="3" t="n">
-        <v>0.638733258076041</v>
+        <v>1.157049779910267</v>
       </c>
       <c r="R37" t="n">
         <v>0.0767170384367596</v>
@@ -2638,7 +2638,7 @@
         <v>0.7266319999999999</v>
       </c>
       <c r="Q38" s="3" t="n">
-        <v>0.638733258076041</v>
+        <v>1.157049779910267</v>
       </c>
       <c r="R38" t="n">
         <v>0.0767170384367596</v>
@@ -2694,7 +2694,7 @@
         <v>0.8</v>
       </c>
       <c r="Q39" s="3" t="n">
-        <v>0.4784930261051164</v>
+        <v>0.9201520384433114</v>
       </c>
       <c r="R39" t="n">
         <v>0.1472633162803166</v>
@@ -2750,7 +2750,7 @@
         <v>0.74413</v>
       </c>
       <c r="Q40" s="3" t="n">
-        <v>0.8527980511516221</v>
+        <v>1.516378108953446</v>
       </c>
       <c r="R40" t="n">
         <v>0.09656722333313997</v>
@@ -2806,7 +2806,7 @@
         <v>0.77</v>
       </c>
       <c r="Q41" s="3" t="n">
-        <v>0.8460331487101693</v>
+        <v>1.506642040307112</v>
       </c>
       <c r="R41" t="n">
         <v>0.0352176809563584</v>
@@ -2862,7 +2862,7 @@
         <v>0.757603</v>
       </c>
       <c r="Q42" s="3" t="n">
-        <v>0.4231331142458284</v>
+        <v>0.8164897989250212</v>
       </c>
       <c r="R42" t="n">
         <v>0.2228342109737272</v>
@@ -2918,7 +2918,7 @@
         <v>0.776484</v>
       </c>
       <c r="Q43" s="3" t="n">
-        <v>0.4065417784609112</v>
+        <v>0.8226369723154777</v>
       </c>
       <c r="R43" t="n">
         <v>0.1256230421520718</v>
@@ -2974,7 +2974,7 @@
         <v>0.77</v>
       </c>
       <c r="Q44" s="3" t="n">
-        <v>0.8582848736645433</v>
+        <v>1.535217968277671</v>
       </c>
       <c r="R44" t="n">
         <v>0.02720601594492704</v>
@@ -3030,7 +3030,7 @@
         <v>0.74</v>
       </c>
       <c r="Q45" s="3" t="n">
-        <v>0.7675547898499949</v>
+        <v>1.380080961817654</v>
       </c>
       <c r="R45" t="n">
         <v>0.01595707167941454</v>
@@ -3086,7 +3086,7 @@
         <v>0.77</v>
       </c>
       <c r="Q46" s="3" t="n">
-        <v>0.440467041313477</v>
+        <v>0.8627064625966099</v>
       </c>
       <c r="R46" t="n">
         <v>0.05814337766711058</v>
@@ -3142,7 +3142,7 @@
         <v>0.841842</v>
       </c>
       <c r="Q47" s="3" t="n">
-        <v>0.7628677312478804</v>
+        <v>1.420266750973085</v>
       </c>
       <c r="R47" t="n">
         <v>0.1131206969732151</v>
@@ -3198,7 +3198,7 @@
         <v>0.841842</v>
       </c>
       <c r="Q48" s="3" t="n">
-        <v>0.7628677312478804</v>
+        <v>1.420266750973085</v>
       </c>
       <c r="R48" t="n">
         <v>0.1131206969732151</v>
@@ -3254,7 +3254,7 @@
         <v>0.87</v>
       </c>
       <c r="Q49" s="3" t="n">
-        <v>0.6423787840647773</v>
+        <v>1.234228002760053</v>
       </c>
       <c r="R49" t="n">
         <v>0.2165786356227843</v>
@@ -3310,7 +3310,7 @@
         <v>0.88</v>
       </c>
       <c r="Q50" s="3" t="n">
-        <v>0.4311738188042931</v>
+        <v>0.9014348176269065</v>
       </c>
       <c r="R50" t="n">
         <v>0.2860097255552455</v>
@@ -3366,7 +3366,7 @@
         <v>0.848675</v>
       </c>
       <c r="Q51" s="3" t="n">
-        <v>0.7509786365939464</v>
+        <v>1.417541627563252</v>
       </c>
       <c r="R51" t="n">
         <v>0.1492879722617396</v>
@@ -3422,7 +3422,7 @@
         <v>0.844852</v>
       </c>
       <c r="Q52" s="3" t="n">
-        <v>0.801501182634099</v>
+        <v>1.484563724091384</v>
       </c>
       <c r="R52" t="n">
         <v>0.05116830388656043</v>
@@ -3478,7 +3478,7 @@
         <v>0.963515</v>
       </c>
       <c r="Q53" s="3" t="n">
-        <v>0.3639498627094521</v>
+        <v>0.8839610806037723</v>
       </c>
       <c r="R53" t="n">
         <v>0.2680494911224468</v>
@@ -3534,7 +3534,7 @@
         <v>0.782479</v>
       </c>
       <c r="Q54" s="3" t="n">
-        <v>0.5830139874015356</v>
+        <v>1.102568633308624</v>
       </c>
       <c r="R54" t="n">
         <v>0.06661906649581383</v>
@@ -3587,7 +3587,7 @@
         <v>0.782479</v>
       </c>
       <c r="Q55" s="3" t="n">
-        <v>0.5830139874015356</v>
+        <v>1.102568633308624</v>
       </c>
       <c r="R55" t="n">
         <v>0.06661906649581383</v>
@@ -3643,7 +3643,7 @@
         <v>0.74982</v>
       </c>
       <c r="Q56" s="3" t="n">
-        <v>0.5505815501150764</v>
+        <v>1.033524097456652</v>
       </c>
       <c r="R56" t="n">
         <v>0.2277199720930105</v>
@@ -3699,7 +3699,7 @@
         <v>0.8</v>
       </c>
       <c r="Q57" s="3" t="n">
-        <v>0.7275928301762715</v>
+        <v>1.342540001201114</v>
       </c>
       <c r="R57" t="n">
         <v>0.1669777466970116</v>
@@ -3755,7 +3755,7 @@
         <v>0.8</v>
       </c>
       <c r="Q58" s="3" t="n">
-        <v>0.7275928301762715</v>
+        <v>1.342540001201114</v>
       </c>
       <c r="R58" t="n">
         <v>0.1669777466970116</v>
@@ -3811,7 +3811,7 @@
         <v>0.96</v>
       </c>
       <c r="Q59" s="3" t="n">
-        <v>0.842554396475881</v>
+        <v>1.626298417461924</v>
       </c>
       <c r="R59" t="n">
         <v>0.1017032808558144</v>
@@ -3867,7 +3867,7 @@
         <v>0.962324</v>
       </c>
       <c r="Q60" s="3" t="n">
-        <v>0.842554396475881</v>
+        <v>1.626298417461924</v>
       </c>
       <c r="R60" t="n">
         <v>0.1017032808558144</v>
@@ -3923,7 +3923,7 @@
         <v>1.02607</v>
       </c>
       <c r="Q61" s="3" t="n">
-        <v>0.4604547707874415</v>
+        <v>1.183025290588741</v>
       </c>
       <c r="R61" t="n">
         <v>0.8241668035706786</v>
@@ -3979,7 +3979,7 @@
         <v>1.02607</v>
       </c>
       <c r="Q62" s="3" t="n">
-        <v>0.4604547707874415</v>
+        <v>1.183025290588741</v>
       </c>
       <c r="R62" t="n">
         <v>0.8241668035706786</v>
@@ -4032,7 +4032,7 @@
         <v>1.02607</v>
       </c>
       <c r="Q63" s="3" t="n">
-        <v>0.4604547707874415</v>
+        <v>1.183025290588741</v>
       </c>
       <c r="R63" t="n">
         <v>0.8241668035706786</v>
@@ -4088,7 +4088,7 @@
         <v>1.02</v>
       </c>
       <c r="Q64" s="3" t="n">
-        <v>0.9064552235095198</v>
+        <v>1.77076379929166</v>
       </c>
       <c r="R64" t="n">
         <v>0.05708224099375498</v>
@@ -4144,7 +4144,7 @@
         <v>1.13</v>
       </c>
       <c r="Q65" s="3" t="n">
-        <v>0.9086312583242271</v>
+        <v>1.822544105549942</v>
       </c>
       <c r="R65" t="n">
         <v>0.06928742029234983</v>
@@ -4200,7 +4200,7 @@
         <v>1.03</v>
       </c>
       <c r="Q66" s="3" t="n">
-        <v>0.8937733752542706</v>
+        <v>1.776874771529581</v>
       </c>
       <c r="R66" t="n">
         <v>0.09064358833580949</v>
@@ -4256,7 +4256,7 @@
         <v>1.15</v>
       </c>
       <c r="Q67" s="3" t="n">
-        <v>0.5682507800699519</v>
+        <v>1.435841770397525</v>
       </c>
       <c r="R67" t="n">
         <v>0.5469902615930315</v>
@@ -4312,7 +4312,7 @@
         <v>1.12993</v>
       </c>
       <c r="Q68" s="3" t="n">
-        <v>0.7181866415369055</v>
+        <v>1.589191432361864</v>
       </c>
       <c r="R68" t="n">
         <v>0.05173693479333623</v>
@@ -4368,7 +4368,7 @@
         <v>1.12993</v>
       </c>
       <c r="Q69" s="3" t="n">
-        <v>0.7181866415369055</v>
+        <v>1.589191432361864</v>
       </c>
       <c r="R69" t="n">
         <v>0.05173693479333623</v>
@@ -4424,7 +4424,7 @@
         <v>1.33</v>
       </c>
       <c r="Q70" s="3" t="n">
-        <v>0.9532128040208352</v>
+        <v>2.099615239697236</v>
       </c>
       <c r="R70" t="n">
         <v>0.0118387871337529</v>
@@ -4480,7 +4480,7 @@
         <v>1.19</v>
       </c>
       <c r="Q71" s="3" t="n">
-        <v>0.9715889119731532</v>
+        <v>2.012620944277857</v>
       </c>
       <c r="R71" t="n">
         <v>0.01731301595994347</v>
@@ -4536,7 +4536,7 @@
         <v>1.09843</v>
       </c>
       <c r="Q72" s="3" t="n">
-        <v>0.7994076233898318</v>
+        <v>1.709403743219913</v>
       </c>
       <c r="R72" t="n">
         <v>0.1616304778941326</v>
@@ -4592,7 +4592,7 @@
         <v>1.09843</v>
       </c>
       <c r="Q73" s="3" t="n">
-        <v>0.7994076233898318</v>
+        <v>1.709403743219913</v>
       </c>
       <c r="R73" t="n">
         <v>0.1616304778941326</v>
@@ -4648,7 +4648,7 @@
         <v>1.22568</v>
       </c>
       <c r="Q74" s="3" t="n">
-        <v>1.176253721254392</v>
+        <v>2.345782205913604</v>
       </c>
       <c r="R74" t="n">
         <v>0.07805369350328827</v>
@@ -4704,7 +4704,7 @@
         <v>1.2845</v>
       </c>
       <c r="Q75" s="3" t="n">
-        <v>3.195893511237676</v>
+        <v>5.691327750389669</v>
       </c>
       <c r="R75" t="n">
         <v>0.08132008275074698</v>
@@ -4760,7 +4760,7 @@
         <v>1.28</v>
       </c>
       <c r="Q76" s="3" t="n">
-        <v>3.195893511237676</v>
+        <v>5.691327750389669</v>
       </c>
       <c r="R76" t="n">
         <v>0.08132008275074698</v>
@@ -4816,7 +4816,7 @@
         <v>1.2845</v>
       </c>
       <c r="Q77" s="3" t="n">
-        <v>3.195893511237676</v>
+        <v>5.691327750389669</v>
       </c>
       <c r="R77" t="n">
         <v>0.08132008275074698</v>
@@ -4872,7 +4872,7 @@
         <v>1.42717</v>
       </c>
       <c r="Q78" s="3" t="n">
-        <v>6.024879354419458</v>
+        <v>10.54475952976137</v>
       </c>
       <c r="R78" t="n">
         <v>0.09557954007745355</v>
@@ -4928,7 +4928,7 @@
         <v>1.42717</v>
       </c>
       <c r="Q79" s="3" t="n">
-        <v>6.024879354419458</v>
+        <v>10.54475952976137</v>
       </c>
       <c r="R79" t="n">
         <v>0.09557954007745355</v>
@@ -4967,7 +4967,7 @@
         <v>154.124</v>
       </c>
       <c r="Q80" s="3" t="n">
-        <v>35.71169791451638</v>
+        <v>61.86865244577595</v>
       </c>
       <c r="R80" t="n">
         <v>0.0305854259260738</v>

</xml_diff>

<commit_message>
fix histogram not updated after reloading dataset
</commit_message>
<xml_diff>
--- a/results/GAIA_TESS_candidate_matches.xlsx
+++ b/results/GAIA_TESS_candidate_matches.xlsx
@@ -622,7 +622,7 @@
         <v>0.618173</v>
       </c>
       <c r="Q2" s="3" t="n">
-        <v>0.7902558828894091</v>
+        <v>1.033196630495687</v>
       </c>
       <c r="R2" t="n">
         <v>0.1536852942719399</v>
@@ -678,7 +678,7 @@
         <v>0.63</v>
       </c>
       <c r="Q3" s="3" t="n">
-        <v>1.743539432563141</v>
+        <v>1.897036734533635</v>
       </c>
       <c r="R3" t="n">
         <v>0.08769119345162939</v>
@@ -734,7 +734,7 @@
         <v>0.7017099999999999</v>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>1.059534344419636</v>
+        <v>1.245846174113728</v>
       </c>
       <c r="R4" t="n">
         <v>0.01821666933803688</v>
@@ -790,7 +790,7 @@
         <v>0.71</v>
       </c>
       <c r="Q5" s="3" t="n">
-        <v>1.65695721791391</v>
+        <v>1.784451737247451</v>
       </c>
       <c r="R5" t="n">
         <v>0.03110876237070922</v>
@@ -846,7 +846,7 @@
         <v>0.626722</v>
       </c>
       <c r="Q6" s="3" t="n">
-        <v>1.627954212787946</v>
+        <v>1.757553896613831</v>
       </c>
       <c r="R6" t="n">
         <v>0.05933370243670238</v>
@@ -902,7 +902,7 @@
         <v>0.636572</v>
       </c>
       <c r="Q7" s="3" t="n">
-        <v>2.161818741545839</v>
+        <v>2.267803543469689</v>
       </c>
       <c r="R7" t="n">
         <v>0.07251061220725062</v>
@@ -958,7 +958,7 @@
         <v>0.6634139999999999</v>
       </c>
       <c r="Q8" s="3" t="n">
-        <v>1.373786090337297</v>
+        <v>1.535174538115806</v>
       </c>
       <c r="R8" t="n">
         <v>0.04285830752449767</v>
@@ -1008,7 +1008,7 @@
         <v>0.88</v>
       </c>
       <c r="Q9" s="3" t="n">
-        <v>1.266231092040509</v>
+        <v>1.439726994580897</v>
       </c>
       <c r="R9" t="n">
         <v>0.1596334725227671</v>
@@ -1064,7 +1064,7 @@
         <v>0.6307199999999999</v>
       </c>
       <c r="Q10" s="3" t="n">
-        <v>2.282167123690875</v>
+        <v>2.402440918079677</v>
       </c>
       <c r="R10" t="n">
         <v>0.04323476018011795</v>
@@ -1120,7 +1120,7 @@
         <v>0.63</v>
       </c>
       <c r="Q11" s="3" t="n">
-        <v>2.282167123690875</v>
+        <v>2.402440918079677</v>
       </c>
       <c r="R11" t="n">
         <v>0.04323476018011795</v>
@@ -1176,7 +1176,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="Q12" s="3" t="n">
-        <v>1.205326888273188</v>
+        <v>1.443841293612757</v>
       </c>
       <c r="R12" t="n">
         <v>0.1692002171172093</v>
@@ -1232,7 +1232,7 @@
         <v>0.732115</v>
       </c>
       <c r="Q13" s="3" t="n">
-        <v>0.8408621631098551</v>
+        <v>1.211275628093407</v>
       </c>
       <c r="R13" t="n">
         <v>0.1818675256393356</v>
@@ -1288,7 +1288,7 @@
         <v>0.63</v>
       </c>
       <c r="Q14" s="3" t="n">
-        <v>1.0925362451314</v>
+        <v>1.309435688241485</v>
       </c>
       <c r="R14" t="n">
         <v>0.2166081726537622</v>
@@ -1344,7 +1344,7 @@
         <v>0.64</v>
       </c>
       <c r="Q15" s="3" t="n">
-        <v>1.1181380300198</v>
+        <v>1.384102258224339</v>
       </c>
       <c r="R15" t="n">
         <v>0.1166629664479221</v>
@@ -1400,7 +1400,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="Q16" s="3" t="n">
-        <v>1.928498791447363</v>
+        <v>2.090989106311385</v>
       </c>
       <c r="R16" t="n">
         <v>0.06653290396318375</v>
@@ -1456,7 +1456,7 @@
         <v>0.77</v>
       </c>
       <c r="Q17" s="3" t="n">
-        <v>0.7050657275740375</v>
+        <v>1.264788290313442</v>
       </c>
       <c r="R17" t="n">
         <v>0.1449687993748953</v>
@@ -1512,7 +1512,7 @@
         <v>0.77</v>
       </c>
       <c r="Q18" s="3" t="n">
-        <v>0.7050657275740375</v>
+        <v>1.264788290313442</v>
       </c>
       <c r="R18" t="n">
         <v>0.1449687993748953</v>
@@ -1568,7 +1568,7 @@
         <v>0.71</v>
       </c>
       <c r="Q19" s="3" t="n">
-        <v>1.517865485656713</v>
+        <v>1.79763062483054</v>
       </c>
       <c r="R19" t="n">
         <v>0.04668015033414173</v>
@@ -1624,7 +1624,7 @@
         <v>0.590924</v>
       </c>
       <c r="Q20" s="3" t="n">
-        <v>2.099223907159651</v>
+        <v>2.185032813561829</v>
       </c>
       <c r="R20" t="n">
         <v>0.1022963165103159</v>
@@ -1680,7 +1680,7 @@
         <v>0.701499</v>
       </c>
       <c r="Q21" s="3" t="n">
-        <v>0.5761162700503707</v>
+        <v>1.251277561671179</v>
       </c>
       <c r="R21" t="n">
         <v>0.2489958576576189</v>
@@ -1736,7 +1736,7 @@
         <v>0.622512</v>
       </c>
       <c r="Q22" s="3" t="n">
-        <v>1.184954404382703</v>
+        <v>1.539342568313268</v>
       </c>
       <c r="R22" t="n">
         <v>0.2100230324201724</v>
@@ -1792,7 +1792,7 @@
         <v>0.75</v>
       </c>
       <c r="Q23" s="3" t="n">
-        <v>0.6056323786844908</v>
+        <v>1.194339638421116</v>
       </c>
       <c r="R23" t="n">
         <v>0.03576864546243089</v>
@@ -1848,7 +1848,7 @@
         <v>0.704768</v>
       </c>
       <c r="Q24" s="3" t="n">
-        <v>1.241545346976267</v>
+        <v>1.633643190573729</v>
       </c>
       <c r="R24" t="n">
         <v>0.1440519013547189</v>
@@ -1904,7 +1904,7 @@
         <v>0.693766</v>
       </c>
       <c r="Q25" s="3" t="n">
-        <v>0.8936552115002135</v>
+        <v>1.342818542634564</v>
       </c>
       <c r="R25" t="n">
         <v>0.01559139926063062</v>
@@ -1960,7 +1960,7 @@
         <v>0.74</v>
       </c>
       <c r="Q26" s="3" t="n">
-        <v>1.128211929288773</v>
+        <v>1.556506674803845</v>
       </c>
       <c r="R26" t="n">
         <v>0.06379238266733318</v>
@@ -2016,7 +2016,7 @@
         <v>0.68</v>
       </c>
       <c r="Q27" s="3" t="n">
-        <v>1.650127957691832</v>
+        <v>1.939346032482382</v>
       </c>
       <c r="R27" t="n">
         <v>0.1915281956726753</v>
@@ -2072,7 +2072,7 @@
         <v>0.76</v>
       </c>
       <c r="Q28" s="3" t="n">
-        <v>0.9663749523476942</v>
+        <v>1.523639546448364</v>
       </c>
       <c r="R28" t="n">
         <v>0.131139051935956</v>
@@ -2128,7 +2128,7 @@
         <v>0.7775840000000001</v>
       </c>
       <c r="Q29" s="3" t="n">
-        <v>1.018507941129634</v>
+        <v>1.533943525003013</v>
       </c>
       <c r="R29" t="n">
         <v>0.02743089734967181</v>
@@ -2184,7 +2184,7 @@
         <v>0.751037</v>
       </c>
       <c r="Q30" s="3" t="n">
-        <v>1.195614194869303</v>
+        <v>1.650922393499214</v>
       </c>
       <c r="R30" t="n">
         <v>0.01675017502121713</v>
@@ -2240,7 +2240,7 @@
         <v>0.751037</v>
       </c>
       <c r="Q31" s="3" t="n">
-        <v>1.195614194869303</v>
+        <v>1.650922393499214</v>
       </c>
       <c r="R31" t="n">
         <v>0.01675017502121713</v>
@@ -2296,7 +2296,7 @@
         <v>0.750598</v>
       </c>
       <c r="Q32" s="3" t="n">
-        <v>0.2670928632313241</v>
+        <v>1.296420910492415</v>
       </c>
       <c r="R32" t="n">
         <v>1.046469990099852</v>
@@ -2352,7 +2352,7 @@
         <v>0.75</v>
       </c>
       <c r="Q33" s="3" t="n">
-        <v>0.2670928632313241</v>
+        <v>1.296420910492415</v>
       </c>
       <c r="R33" t="n">
         <v>1.046469990099852</v>
@@ -2408,7 +2408,7 @@
         <v>0.74413</v>
       </c>
       <c r="Q34" s="3" t="n">
-        <v>1.116655495291831</v>
+        <v>1.612698332942558</v>
       </c>
       <c r="R34" t="n">
         <v>0.09656722333313997</v>
@@ -2464,7 +2464,7 @@
         <v>0.6959920000000001</v>
       </c>
       <c r="Q35" s="3" t="n">
-        <v>0.9180746601776205</v>
+        <v>1.450838758676033</v>
       </c>
       <c r="R35" t="n">
         <v>0.05872196175686627</v>
@@ -2520,7 +2520,7 @@
         <v>0.776484</v>
       </c>
       <c r="Q36" s="3" t="n">
-        <v>0.4972489485376618</v>
+        <v>1.467604750719693</v>
       </c>
       <c r="R36" t="n">
         <v>0.1256230421520718</v>
@@ -2576,7 +2576,7 @@
         <v>0.77</v>
       </c>
       <c r="Q37" s="3" t="n">
-        <v>1.113358310196863</v>
+        <v>1.689140930763304</v>
       </c>
       <c r="R37" t="n">
         <v>0.02720601594492704</v>
@@ -2632,7 +2632,7 @@
         <v>0.78</v>
       </c>
       <c r="Q38" s="3" t="n">
-        <v>0.9396839689860219</v>
+        <v>1.63699196957063</v>
       </c>
       <c r="R38" t="n">
         <v>0.1100198261051309</v>
@@ -2688,7 +2688,7 @@
         <v>0.77</v>
       </c>
       <c r="Q39" s="3" t="n">
-        <v>0.5412196444315075</v>
+        <v>1.451460227890586</v>
       </c>
       <c r="R39" t="n">
         <v>0.05814337766711058</v>
@@ -2744,7 +2744,7 @@
         <v>0.7721479999999999</v>
       </c>
       <c r="Q40" s="3" t="n">
-        <v>0.9481211214084003</v>
+        <v>1.726090802103506</v>
       </c>
       <c r="R40" t="n">
         <v>0.05926071698556891</v>
@@ -2800,7 +2800,7 @@
         <v>0.77</v>
       </c>
       <c r="Q41" s="3" t="n">
-        <v>0.9481211214084003</v>
+        <v>1.726090802103506</v>
       </c>
       <c r="R41" t="n">
         <v>0.05926071698556891</v>
@@ -2856,7 +2856,7 @@
         <v>0.77</v>
       </c>
       <c r="Q42" s="3" t="n">
-        <v>0.9481211214084003</v>
+        <v>1.726090802103506</v>
       </c>
       <c r="R42" t="n">
         <v>0.05926071698556891</v>
@@ -2912,7 +2912,7 @@
         <v>0.88</v>
       </c>
       <c r="Q43" s="3" t="n">
-        <v>0.5168819078281685</v>
+        <v>1.704998939529603</v>
       </c>
       <c r="R43" t="n">
         <v>0.2860097255552455</v>
@@ -2968,7 +2968,7 @@
         <v>0.844852</v>
       </c>
       <c r="Q44" s="3" t="n">
-        <v>1.024745179501231</v>
+        <v>1.951846748730099</v>
       </c>
       <c r="R44" t="n">
         <v>0.05116830388656043</v>
@@ -3024,7 +3024,7 @@
         <v>0.963515</v>
       </c>
       <c r="Q45" s="3" t="n">
-        <v>0.4015502513867581</v>
+        <v>1.977480319599974</v>
       </c>
       <c r="R45" t="n">
         <v>0.2680494911224468</v>
@@ -3080,7 +3080,7 @@
         <v>0.823126</v>
       </c>
       <c r="Q46" s="3" t="n">
-        <v>0.8269642916723454</v>
+        <v>1.813585229043661</v>
       </c>
       <c r="R46" t="n">
         <v>0.06164093083342125</v>
@@ -3136,7 +3136,7 @@
         <v>0.782479</v>
       </c>
       <c r="Q47" s="3" t="n">
-        <v>0.7320316021428864</v>
+        <v>1.636354764225714</v>
       </c>
       <c r="R47" t="n">
         <v>0.06661906649581383</v>
@@ -3189,7 +3189,7 @@
         <v>0.782479</v>
       </c>
       <c r="Q48" s="3" t="n">
-        <v>0.7320316021428864</v>
+        <v>1.636354764225714</v>
       </c>
       <c r="R48" t="n">
         <v>0.06661906649581383</v>
@@ -3245,7 +3245,7 @@
         <v>0.735511</v>
       </c>
       <c r="Q49" s="3" t="n">
-        <v>0.8686322884856515</v>
+        <v>1.679049255710149</v>
       </c>
       <c r="R49" t="n">
         <v>0.03779261048666958</v>
@@ -3301,7 +3301,7 @@
         <v>1.1485</v>
       </c>
       <c r="Q50" s="3" t="n">
-        <v>0.7588600719679252</v>
+        <v>3.617164992432295</v>
       </c>
       <c r="R50" t="n">
         <v>0.03260486313902574</v>
@@ -3357,7 +3357,7 @@
         <v>0.9</v>
       </c>
       <c r="Q51" s="3" t="n">
-        <v>1.064324053827933</v>
+        <v>2.188020963138853</v>
       </c>
       <c r="R51" t="n">
         <v>0.05635993153899293</v>
@@ -3413,7 +3413,7 @@
         <v>0.96</v>
       </c>
       <c r="Q52" s="3" t="n">
-        <v>1.061668841907705</v>
+        <v>2.45663422781619</v>
       </c>
       <c r="R52" t="n">
         <v>0.1017032808558144</v>
@@ -3469,7 +3469,7 @@
         <v>0.962324</v>
       </c>
       <c r="Q53" s="3" t="n">
-        <v>1.061668841907705</v>
+        <v>2.45663422781619</v>
       </c>
       <c r="R53" t="n">
         <v>0.1017032808558144</v>
@@ -3525,7 +3525,7 @@
         <v>0.945408</v>
       </c>
       <c r="Q54" s="3" t="n">
-        <v>1.06975163481739</v>
+        <v>2.477646543958159</v>
       </c>
       <c r="R54" t="n">
         <v>0.1092036781983211</v>
@@ -3581,7 +3581,7 @@
         <v>1.0159301</v>
       </c>
       <c r="Q55" s="3" t="n">
-        <v>0.8694920586555916</v>
+        <v>2.723091978666176</v>
       </c>
       <c r="R55" t="n">
         <v>0.05216827044224256</v>
@@ -3637,7 +3637,7 @@
         <v>1.26</v>
       </c>
       <c r="Q56" s="3" t="n">
-        <v>0.7448828008906113</v>
+        <v>3.487009655055755</v>
       </c>
       <c r="R56" t="n">
         <v>0.05203226078176128</v>
@@ -3693,7 +3693,7 @@
         <v>1.12993</v>
       </c>
       <c r="Q57" s="3" t="n">
-        <v>0.8497931073350418</v>
+        <v>3.165630025183241</v>
       </c>
       <c r="R57" t="n">
         <v>0.05173693479333623</v>
@@ -3749,7 +3749,7 @@
         <v>1.12993</v>
       </c>
       <c r="Q58" s="3" t="n">
-        <v>0.8497931073350418</v>
+        <v>3.165630025183241</v>
       </c>
       <c r="R58" t="n">
         <v>0.05173693479333623</v>
@@ -3805,7 +3805,7 @@
         <v>1.12506</v>
       </c>
       <c r="Q59" s="3" t="n">
-        <v>0.9641417894894451</v>
+        <v>3.198652056791207</v>
       </c>
       <c r="R59" t="n">
         <v>0.08438831092999147</v>
@@ -3861,7 +3861,7 @@
         <v>1.19</v>
       </c>
       <c r="Q60" s="3" t="n">
-        <v>1.191718672573501</v>
+        <v>3.571290677517552</v>
       </c>
       <c r="R60" t="n">
         <v>0.01731301595994347</v>
@@ -3917,7 +3917,7 @@
         <v>1.22568</v>
       </c>
       <c r="Q61" s="3" t="n">
-        <v>1.457313216125925</v>
+        <v>3.824617860709115</v>
       </c>
       <c r="R61" t="n">
         <v>0.07805369350328827</v>
@@ -3973,7 +3973,7 @@
         <v>1.42717</v>
       </c>
       <c r="Q62" s="3" t="n">
-        <v>7.661122693237147</v>
+        <v>8.937750311733469</v>
       </c>
       <c r="R62" t="n">
         <v>0.09557954007745355</v>
@@ -4029,7 +4029,7 @@
         <v>1.42717</v>
       </c>
       <c r="Q63" s="3" t="n">
-        <v>7.661122693237147</v>
+        <v>8.937750311733469</v>
       </c>
       <c r="R63" t="n">
         <v>0.09557954007745355</v>

</xml_diff>

<commit_message>
major update: code structure clean up
</commit_message>
<xml_diff>
--- a/results/GAIA_TESS_candidate_matches.xlsx
+++ b/results/GAIA_TESS_candidate_matches.xlsx
@@ -622,7 +622,7 @@
         <v>0.71</v>
       </c>
       <c r="Q2" s="3" t="n">
-        <v>1.019880171092267</v>
+        <v>0.5747214936203638</v>
       </c>
       <c r="R2" t="n">
         <v>0.216873501781118</v>
@@ -678,7 +678,7 @@
         <v>0.71</v>
       </c>
       <c r="Q3" s="3" t="n">
-        <v>1.019880171092267</v>
+        <v>0.5747214936203638</v>
       </c>
       <c r="R3" t="n">
         <v>0.216873501781118</v>
@@ -734,7 +734,7 @@
         <v>0.630715</v>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>0.8180441313395623</v>
+        <v>0.4573291322971118</v>
       </c>
       <c r="R4" t="n">
         <v>0.3529309609610866</v>
@@ -790,7 +790,7 @@
         <v>0.630715</v>
       </c>
       <c r="Q5" s="3" t="n">
-        <v>0.8180441313395623</v>
+        <v>0.4573291322971118</v>
       </c>
       <c r="R5" t="n">
         <v>0.3529309609610866</v>
@@ -846,7 +846,7 @@
         <v>0.630715</v>
       </c>
       <c r="Q6" s="3" t="n">
-        <v>0.8180441313395623</v>
+        <v>0.4573291322971118</v>
       </c>
       <c r="R6" t="n">
         <v>0.3529309609610866</v>
@@ -902,7 +902,7 @@
         <v>0.8</v>
       </c>
       <c r="Q7" s="3" t="n">
-        <v>1.597062214762744</v>
+        <v>0.9099502856655908</v>
       </c>
       <c r="R7" t="n">
         <v>0.1472633162803166</v>
@@ -958,7 +958,7 @@
         <v>0.757603</v>
       </c>
       <c r="Q8" s="3" t="n">
-        <v>1.208666246344946</v>
+        <v>0.6689697604315441</v>
       </c>
       <c r="R8" t="n">
         <v>0.2228342109737272</v>
@@ -1014,7 +1014,7 @@
         <v>0.88</v>
       </c>
       <c r="Q9" s="3" t="n">
-        <v>1.719165057290658</v>
+        <v>0.8326105656603114</v>
       </c>
       <c r="R9" t="n">
         <v>0.2860097255552455</v>
@@ -1070,7 +1070,7 @@
         <v>1.02607</v>
       </c>
       <c r="Q10" s="3" t="n">
-        <v>2.209049609459966</v>
+        <v>0.8786003547184101</v>
       </c>
       <c r="R10" t="n">
         <v>0.8241668035706786</v>
@@ -1126,7 +1126,7 @@
         <v>1.02607</v>
       </c>
       <c r="Q11" s="3" t="n">
-        <v>2.209049609459966</v>
+        <v>0.8786003547184101</v>
       </c>
       <c r="R11" t="n">
         <v>0.8241668035706786</v>
@@ -1179,7 +1179,7 @@
         <v>1.02607</v>
       </c>
       <c r="Q12" s="3" t="n">
-        <v>2.209049609459966</v>
+        <v>0.8786003547184101</v>
       </c>
       <c r="R12" t="n">
         <v>0.8241668035706786</v>
@@ -1235,7 +1235,7 @@
         <v>1.03</v>
       </c>
       <c r="Q13" s="3" t="n">
-        <v>2.503660604420008</v>
+        <v>1.386957062992251</v>
       </c>
       <c r="R13" t="n">
         <v>0.09064358833580949</v>
@@ -1291,7 +1291,7 @@
         <v>1.33</v>
       </c>
       <c r="Q14" s="3" t="n">
-        <v>3.530285645418739</v>
+        <v>1.692375571059443</v>
       </c>
       <c r="R14" t="n">
         <v>0.0118387871337529</v>
@@ -1347,7 +1347,7 @@
         <v>1.09843</v>
       </c>
       <c r="Q15" s="3" t="n">
-        <v>3.157297112102346</v>
+        <v>1.546870014982985</v>
       </c>
       <c r="R15" t="n">
         <v>0.1616304778941326</v>
@@ -1403,7 +1403,7 @@
         <v>1.09843</v>
       </c>
       <c r="Q16" s="3" t="n">
-        <v>3.157297112102346</v>
+        <v>1.546870014982985</v>
       </c>
       <c r="R16" t="n">
         <v>0.1616304778941326</v>
@@ -1459,7 +1459,7 @@
         <v>1.2845</v>
       </c>
       <c r="Q17" s="3" t="n">
-        <v>6.397373081970478</v>
+        <v>4.872880388587285</v>
       </c>
       <c r="R17" t="n">
         <v>0.08132008275074698</v>
@@ -1515,7 +1515,7 @@
         <v>1.28</v>
       </c>
       <c r="Q18" s="3" t="n">
-        <v>6.397373081970478</v>
+        <v>4.872880388587285</v>
       </c>
       <c r="R18" t="n">
         <v>0.08132008275074698</v>
@@ -1571,7 +1571,7 @@
         <v>1.2845</v>
       </c>
       <c r="Q19" s="3" t="n">
-        <v>6.397373081970478</v>
+        <v>4.872880388587285</v>
       </c>
       <c r="R19" t="n">
         <v>0.08132008275074698</v>
@@ -1627,7 +1627,7 @@
         <v>1.42717</v>
       </c>
       <c r="Q20" s="3" t="n">
-        <v>12.41551009314516</v>
+        <v>10.16437674197399</v>
       </c>
       <c r="R20" t="n">
         <v>0.09557954007745355</v>
@@ -1683,7 +1683,7 @@
         <v>1.42717</v>
       </c>
       <c r="Q21" s="3" t="n">
-        <v>12.41551009314516</v>
+        <v>10.16437674197399</v>
       </c>
       <c r="R21" t="n">
         <v>0.09557954007745355</v>

</xml_diff>